<commit_message>
Time units were wrong.
If (runtime) is really returning microseconds then I reporting seconds
and not milliseconds since I am / by a million.  I updated time unit
labels.
</commit_message>
<xml_diff>
--- a/ryan_p/EX_1_22_Analysis.xlsx
+++ b/ryan_p/EX_1_22_Analysis.xlsx
@@ -11,10 +11,6 @@
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -143,11 +139,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="142352768"/>
-        <c:axId val="142374016"/>
+        <c:axId val="210322560"/>
+        <c:axId val="212447616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142352768"/>
+        <c:axId val="210322560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -156,7 +152,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142374016"/>
+        <c:crossAx val="212447616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -164,7 +160,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142374016"/>
+        <c:axId val="212447616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -182,7 +178,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>ms</a:t>
+                  <a:t>Seconds</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -194,7 +190,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142352768"/>
+        <c:crossAx val="210322560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -221,10 +217,10 @@
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -536,7 +532,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>